<commit_message>
<feat> : add classdiagram and update schedule
</commit_message>
<xml_diff>
--- a/Documents/Kế Hoạch Thực Hiện.xlsx
+++ b/Documents/Kế Hoạch Thực Hiện.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HeThongQuanLyThuVien\Docunents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HeThongQuanLyThuVien\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5EA5A0D-08E3-4A7B-9401-B1C6E6FEDDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039B1D68-1FC6-4C64-BC53-449627B2E81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{13AE7556-501D-443D-8103-62FAEB67678B}"/>
   </bookViews>
@@ -520,7 +520,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -591,7 +591,7 @@
       <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -600,8 +600,8 @@
       <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -610,6 +610,8 @@
       <c r="B6" t="s">
         <v>15</v>
       </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -618,6 +620,8 @@
       <c r="B7" t="s">
         <v>16</v>
       </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -626,6 +630,9 @@
       <c r="B8" t="s">
         <v>17</v>
       </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -634,6 +641,8 @@
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -642,6 +651,8 @@
       <c r="B10" t="s">
         <v>19</v>
       </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -650,6 +661,7 @@
       <c r="B11" t="s">
         <v>20</v>
       </c>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -666,6 +678,8 @@
       <c r="B13" t="s">
         <v>22</v>
       </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -674,6 +688,9 @@
       <c r="B14" t="s">
         <v>23</v>
       </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">

</xml_diff>